<commit_message>
Theo mit Bilder plus BFEld
</commit_message>
<xml_diff>
--- a/BFeld.xlsx
+++ b/BFeld.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jlvi2\OneDrive\Desktop\Physik\Fortgeschr. Praktikum\V46----Faraday-Effekt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EBD77819-4995-41E1-A728-F4A405B5ACB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{88362F7A-CF41-466C-BC2D-20F6A340507F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1095" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{F6D8C6CA-AEC2-41C9-B877-C74D3FBACCE0}"/>
+    <workbookView xWindow="65895" yWindow="5280" windowWidth="14610" windowHeight="15585" xr2:uid="{F6D8C6CA-AEC2-41C9-B877-C74D3FBACCE0}"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="BFeld" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -413,10 +413,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94AD9109-7E0E-493A-B80F-5BD75E64DA96}">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -533,6 +533,14 @@
         <v>204</v>
       </c>
     </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>112</v>
+      </c>
+      <c r="B15">
+        <v>105</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>